<commit_message>
finish user friendly normal time and add forward&rewind button but it's can not work
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -18,39 +18,17 @@
     <sheet name="Video複偵測" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Video複偵測1" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="紗布_少偵測" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="紗布_重複偵測" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="鼻子_重複偵測" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="紗布_重複偵測1" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="紗布_重複偵測2" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="紗布_重複偵測3" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="紗布_少偵測1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="紗布_重複偵測4" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="紗布_重複偵測5" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="鏡頭上血跡" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="紗布_少偵測2" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="鼻子_重複偵測1" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="紗布_少偵測3" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="紗布_少偵測4" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="紗布_少偵測5" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="鏡頭上血跡1" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="紗布_少偵測6" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="紗布_少偵測7" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="紗布_少偵測8" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="紗布_少偵測9" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="紗布_少偵測10" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="紗布_少偵測11" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="紗布_少偵測12" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="紗布_少偵測13" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="紗布_少偵測14" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="紗布_少偵測15" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="紗布_少偵測16" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="紗布_少偵測17" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="紗布_少偵測18" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="紗布_少偵測19" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="try_video" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="紗布_少偵測20" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="紗布_少偵測21" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="try_video1" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="紗布_少偵測1" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="紗布_少偵測2" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="紗布_少偵測3" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="紗布_少偵測4" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="try_video" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="紗布_少偵測5" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="5" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="52" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="53" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="54" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="紗布_少偵測6" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -660,7 +638,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0: 1</t>
+          <t>00: 1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -670,7 +648,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0: 2</t>
+          <t>00: 2</t>
         </is>
       </c>
     </row>
@@ -696,7 +674,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>紗布_重複偵測</t>
+          <t>紗布_少偵測</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -728,22 +706,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0: 1</t>
+          <t>00: 1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0: 4</t>
+          <t>00: 2</t>
         </is>
       </c>
     </row>
@@ -758,7 +736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -769,7 +747,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>鼻子_重複偵測</t>
+          <t>紗布_少偵測</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -790,6 +768,33 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>End Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Interrupt#0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>00: 1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>00: 2</t>
         </is>
       </c>
     </row>
@@ -815,7 +820,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>紗布_重複偵測</t>
+          <t>紗布_少偵測</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -847,22 +852,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0: 1</t>
+          <t>00: 1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0: 4</t>
+          <t>00: 2</t>
         </is>
       </c>
     </row>
@@ -888,7 +893,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>紗布_重複偵測</t>
+          <t>紗布_少偵測</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -920,22 +925,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0: 1</t>
+          <t>00: 01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0: 4</t>
+          <t>00: 02</t>
         </is>
       </c>
     </row>
@@ -950,7 +955,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -961,7 +966,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>紗布_重複偵測</t>
+          <t>try_video</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -993,22 +998,454 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>123</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0: 1</t>
+          <t>00: 04</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>151</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0: 4</t>
+          <t>00: 06</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Interrupt#1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1310</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>00: 48</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1322</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>00: 48</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Interrupt#2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1539</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>00: 56</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1600</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>00: 59</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Interrupt#3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1908</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01: 10</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2066</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>01: 16</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Interrupt#4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2457</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01: 30</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2556</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01: 34</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Interrupt#5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2922</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>01: 47</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2974</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>01: 49</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Interrupt#6</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3164</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>01: 56</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3255</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>01: 59</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Interrupt#7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>3322</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>02: 02</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3333</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>02: 02</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Interrupt#8</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>3519</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>02: 09</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3565</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>02: 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Interrupt#9</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>3635</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>02: 13</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3680</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>02: 15</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Interrupt#10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3786</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>02: 19</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3865</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>02: 22</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Interrupt#11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>3941</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>02: 25</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3988</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>02: 26</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Interrupt#12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>4660</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>02: 51</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4884</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>02: 59</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Interrupt#13</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>4926</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>03: 01</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4971</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>03: 02</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Interrupt#14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5102</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>03: 07</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>5165</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>03: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Interrupt#15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5338</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>03: 16</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>5373</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>03: 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Interrupt#16</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>5835</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>03: 34</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>5877</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>03: 36</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1508,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0: 1</t>
+          <t>00: 01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1081,7 +1518,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0: 2</t>
+          <t>00: 02</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1107,7 +1544,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>紗布_重複偵測</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1128,33 +1565,6 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 37</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 52</t>
         </is>
       </c>
     </row>
@@ -1944,7 +2354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1955,7 +2365,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>紗布_重複偵測</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1976,33 +2386,6 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 37</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 52</t>
         </is>
       </c>
     </row>
@@ -2028,7 +2411,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>鏡頭上血跡</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2063,7 +2446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2074,7 +2457,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>紗布_少偵測</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2095,33 +2478,6 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2503,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>鼻子_重複偵測</t>
+          <t>紗布_少偵測</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2179,433 +2535,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0: 31</t>
+          <t>00: 01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1: 22</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>鏡頭上血跡</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
+          <t>00: 02</t>
         </is>
       </c>
     </row>
@@ -3322,736 +3267,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 30</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1: 2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -4546,1254 +3761,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>try_video</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 4.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>147</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Interrupt#1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1540</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0: 56.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1595</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0: 58.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Interrupt#2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1915</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1: 10.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2065</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1: 16.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Interrupt#3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2457</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1: 30.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2555</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1: 34.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Interrupt#4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2922</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1: 47.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2974</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1: 49.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Interrupt#5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3164</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1: 56.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>3254</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1: 59.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Interrupt#6</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>3322</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2: 2.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>3332</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2: 2.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Interrupt#7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>3519</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2: 9.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>3565</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2: 11.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Interrupt#8</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>3635</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2: 13.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>3679</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2: 15.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Interrupt#9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>3788</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2: 19.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>3862</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2: 22.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Interrupt#10</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>3941</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2: 25.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>3988</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2: 26.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Interrupt#11</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>4660</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2: 51.0</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>4879</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2: 59.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Interrupt#12</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>4926</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>3: 1.0</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>4970</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>3: 2.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Interrupt#13</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>5102</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>3: 7.0</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>5165</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>3: 10.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Interrupt#14</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>5338</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>3: 16.0</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>5373</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>3: 17.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Interrupt#15</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>5839</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>3: 34.0</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>5868</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>3: 35.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>紗布_少偵測</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 1.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 2.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>try_video</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Start Frame #</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>End Frame #</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Interrupt#0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0: 4.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>147</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0: 5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Interrupt#1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1540</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0: 56.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1595</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0: 58.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Interrupt#2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1915</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1: 10.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2065</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1: 16.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Interrupt#3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2457</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1: 30.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2555</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1: 34.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Interrupt#4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2922</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1: 47.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2974</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1: 49.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Interrupt#5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3164</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1: 56.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>3254</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1: 59.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Interrupt#6</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>3322</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2: 2.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>3332</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2: 2.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Interrupt#7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>3519</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2: 9.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>3565</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2: 11.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Interrupt#8</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>3635</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2: 13.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>3679</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2: 15.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Interrupt#9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>3788</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2: 19.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>3862</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2: 22.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Interrupt#10</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>3941</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2: 25.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>3988</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2: 26.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Interrupt#11</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>4660</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2: 51.0</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>4879</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2: 59.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Interrupt#12</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>4926</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>3: 1.0</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>4970</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>3: 2.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Interrupt#13</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>5102</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>3: 7.0</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>5165</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>3: 10.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Interrupt#14</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>5338</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>3: 16.0</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>5373</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>3: 17.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Interrupt#15</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>5839</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>3: 34.0</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>5868</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>3: 35.0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
.txt file revise done
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -37,6 +37,27 @@
     <sheet name="紗布_少偵測8" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="紗布_少偵測9" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="59" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="血肉太白" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="血肉太白1" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="白煙" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="白煙1" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="白煙2" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="白煙3" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="白煙4" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="血肉太白2" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="白煙5" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="白煙6" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="白煙7" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="白煙8" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="白煙9" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="白煙10" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="白煙11" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="血肉太白3" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="白煙12" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="血肉太白4" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="白煙13" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="白煙14" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="血肉太白5" sheetId="52" state="visible" r:id="rId52"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -3724,6 +3745,374 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>血肉太白</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>血肉太白</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>血肉太白</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -4218,6 +4607,466 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>血肉太白</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>血肉太白</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -4744,6 +5593,144 @@
       <c r="F18" s="1" t="inlineStr">
         <is>
           <t>O</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>白煙</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>血肉太白</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start Frame #</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>End Frame #</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>End Time</t>
         </is>
       </c>
     </row>

</xml_diff>